<commit_message>
update data and md summary
</commit_message>
<xml_diff>
--- a/data/Pinnniped_Monitoring_CABR_Data2.xlsx
+++ b/data/Pinnniped_Monitoring_CABR_Data2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\LP_Files\RStudio_Files\cabr_pinniped\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LP_Files\RStudio_Files\cabr_pinniped\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488AB1AF-5EFD-4CFB-A2A8-8578D7A793A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C115F60-4F08-462E-9697-5C1DF17AC241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="14016" xr2:uid="{17D13528-A7EB-4C82-8A74-875F1AEE6115}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="58">
   <si>
     <t>date</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>people too numerous to count</t>
+  </si>
+  <si>
+    <t>parking lot full</t>
   </si>
 </sst>
 </file>
@@ -564,11 +567,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405B0637-EF83-461D-AE7E-5772E674DF6B}">
-  <dimension ref="A1:O109"/>
+  <dimension ref="A1:O124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M110" sqref="M110"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M125" sqref="M125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5464,6 +5467,666 @@
         <v>2</v>
       </c>
     </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A110" s="1">
+        <v>44640</v>
+      </c>
+      <c r="B110" t="s">
+        <v>14</v>
+      </c>
+      <c r="C110">
+        <v>50</v>
+      </c>
+      <c r="D110">
+        <v>4</v>
+      </c>
+      <c r="E110" t="s">
+        <v>15</v>
+      </c>
+      <c r="F110" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G110" s="3">
+        <v>44640.5</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="I110">
+        <v>0</v>
+      </c>
+      <c r="J110">
+        <v>0</v>
+      </c>
+      <c r="K110">
+        <v>0</v>
+      </c>
+      <c r="L110">
+        <v>0</v>
+      </c>
+      <c r="M110">
+        <v>0</v>
+      </c>
+      <c r="N110">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A111" s="1">
+        <v>44640</v>
+      </c>
+      <c r="B111" t="s">
+        <v>14</v>
+      </c>
+      <c r="C111">
+        <v>50</v>
+      </c>
+      <c r="D111">
+        <v>4</v>
+      </c>
+      <c r="E111" t="s">
+        <v>16</v>
+      </c>
+      <c r="F111" s="2">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="G111" s="3">
+        <v>44640.597222222219</v>
+      </c>
+      <c r="H111">
+        <v>0</v>
+      </c>
+      <c r="I111">
+        <v>0</v>
+      </c>
+      <c r="J111">
+        <v>0</v>
+      </c>
+      <c r="K111">
+        <v>0</v>
+      </c>
+      <c r="L111">
+        <v>1</v>
+      </c>
+      <c r="M111">
+        <v>0</v>
+      </c>
+      <c r="N111">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A112" s="1">
+        <v>44640</v>
+      </c>
+      <c r="B112" t="s">
+        <v>14</v>
+      </c>
+      <c r="C112">
+        <v>50</v>
+      </c>
+      <c r="D112">
+        <v>4</v>
+      </c>
+      <c r="E112" t="s">
+        <v>17</v>
+      </c>
+      <c r="F112" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="G112" s="3">
+        <v>44640.625</v>
+      </c>
+      <c r="H112">
+        <v>0</v>
+      </c>
+      <c r="I112">
+        <v>0</v>
+      </c>
+      <c r="J112">
+        <v>0</v>
+      </c>
+      <c r="K112">
+        <v>0</v>
+      </c>
+      <c r="L112">
+        <v>0</v>
+      </c>
+      <c r="M112">
+        <v>0</v>
+      </c>
+      <c r="N112">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A113" s="1">
+        <v>44647</v>
+      </c>
+      <c r="B113" t="s">
+        <v>14</v>
+      </c>
+      <c r="C113">
+        <v>20</v>
+      </c>
+      <c r="D113">
+        <v>3</v>
+      </c>
+      <c r="E113" t="s">
+        <v>15</v>
+      </c>
+      <c r="F113" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G113" s="3">
+        <v>44647.5</v>
+      </c>
+      <c r="H113">
+        <v>0</v>
+      </c>
+      <c r="I113">
+        <v>0</v>
+      </c>
+      <c r="J113">
+        <v>0</v>
+      </c>
+      <c r="K113">
+        <v>0</v>
+      </c>
+      <c r="L113">
+        <v>0</v>
+      </c>
+      <c r="M113">
+        <v>0</v>
+      </c>
+      <c r="O113" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A114" s="1">
+        <v>44647</v>
+      </c>
+      <c r="B114" t="s">
+        <v>14</v>
+      </c>
+      <c r="C114">
+        <v>20</v>
+      </c>
+      <c r="D114">
+        <v>3</v>
+      </c>
+      <c r="E114" t="s">
+        <v>16</v>
+      </c>
+      <c r="F114" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="G114" s="3">
+        <v>44647.541666666664</v>
+      </c>
+      <c r="H114">
+        <v>27</v>
+      </c>
+      <c r="I114">
+        <v>2</v>
+      </c>
+      <c r="J114">
+        <v>0</v>
+      </c>
+      <c r="K114">
+        <v>0</v>
+      </c>
+      <c r="L114">
+        <v>0</v>
+      </c>
+      <c r="M114">
+        <v>0</v>
+      </c>
+      <c r="N114">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A115" s="1">
+        <v>44647</v>
+      </c>
+      <c r="B115" t="s">
+        <v>14</v>
+      </c>
+      <c r="C115">
+        <v>20</v>
+      </c>
+      <c r="D115">
+        <v>3</v>
+      </c>
+      <c r="E115" t="s">
+        <v>17</v>
+      </c>
+      <c r="F115" s="2">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="G115" s="3">
+        <v>44647.569444444445</v>
+      </c>
+      <c r="H115">
+        <v>2</v>
+      </c>
+      <c r="I115">
+        <v>1</v>
+      </c>
+      <c r="J115">
+        <v>0</v>
+      </c>
+      <c r="K115">
+        <v>0</v>
+      </c>
+      <c r="L115">
+        <v>0</v>
+      </c>
+      <c r="M115">
+        <v>0</v>
+      </c>
+      <c r="O115" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A116" s="1">
+        <v>44654</v>
+      </c>
+      <c r="B116" t="s">
+        <v>14</v>
+      </c>
+      <c r="C116">
+        <v>100</v>
+      </c>
+      <c r="D116">
+        <v>4</v>
+      </c>
+      <c r="E116" t="s">
+        <v>15</v>
+      </c>
+      <c r="F116" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G116" s="3">
+        <v>44654.5</v>
+      </c>
+      <c r="H116">
+        <v>0</v>
+      </c>
+      <c r="I116">
+        <v>0</v>
+      </c>
+      <c r="J116">
+        <v>0</v>
+      </c>
+      <c r="K116">
+        <v>0</v>
+      </c>
+      <c r="L116">
+        <v>0</v>
+      </c>
+      <c r="M116">
+        <v>0</v>
+      </c>
+      <c r="N116">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
+        <v>44654</v>
+      </c>
+      <c r="B117" t="s">
+        <v>14</v>
+      </c>
+      <c r="C117">
+        <v>100</v>
+      </c>
+      <c r="D117">
+        <v>4</v>
+      </c>
+      <c r="E117" t="s">
+        <v>16</v>
+      </c>
+      <c r="F117" s="2">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="G117" s="3">
+        <v>44654.652777777781</v>
+      </c>
+      <c r="H117">
+        <v>1</v>
+      </c>
+      <c r="I117">
+        <v>0</v>
+      </c>
+      <c r="J117">
+        <v>0</v>
+      </c>
+      <c r="K117">
+        <v>0</v>
+      </c>
+      <c r="L117">
+        <v>1</v>
+      </c>
+      <c r="M117">
+        <v>0</v>
+      </c>
+      <c r="N117">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A118" s="1">
+        <v>44654</v>
+      </c>
+      <c r="B118" t="s">
+        <v>14</v>
+      </c>
+      <c r="C118">
+        <v>100</v>
+      </c>
+      <c r="D118">
+        <v>4</v>
+      </c>
+      <c r="E118" t="s">
+        <v>17</v>
+      </c>
+      <c r="F118" s="2">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="G118" s="3">
+        <v>44654.631944444445</v>
+      </c>
+      <c r="H118">
+        <v>1</v>
+      </c>
+      <c r="I118">
+        <v>0</v>
+      </c>
+      <c r="J118">
+        <v>0</v>
+      </c>
+      <c r="K118">
+        <v>0</v>
+      </c>
+      <c r="L118">
+        <v>0</v>
+      </c>
+      <c r="M118">
+        <v>0</v>
+      </c>
+      <c r="N118">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A119" s="1">
+        <v>44675</v>
+      </c>
+      <c r="B119" t="s">
+        <v>14</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119">
+        <v>3</v>
+      </c>
+      <c r="E119" t="s">
+        <v>15</v>
+      </c>
+      <c r="F119" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G119" s="3">
+        <v>44675.583333333336</v>
+      </c>
+      <c r="H119">
+        <v>0</v>
+      </c>
+      <c r="I119">
+        <v>0</v>
+      </c>
+      <c r="J119">
+        <v>0</v>
+      </c>
+      <c r="K119">
+        <v>0</v>
+      </c>
+      <c r="L119">
+        <v>0</v>
+      </c>
+      <c r="M119">
+        <v>0</v>
+      </c>
+      <c r="N119">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A120" s="1">
+        <v>44675</v>
+      </c>
+      <c r="B120" t="s">
+        <v>14</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <v>3</v>
+      </c>
+      <c r="E120" t="s">
+        <v>16</v>
+      </c>
+      <c r="F120" s="2">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="G120" s="3">
+        <v>44675.614583333336</v>
+      </c>
+      <c r="H120">
+        <v>13</v>
+      </c>
+      <c r="I120">
+        <v>0</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
+      </c>
+      <c r="K120">
+        <v>0</v>
+      </c>
+      <c r="L120">
+        <v>0</v>
+      </c>
+      <c r="M120">
+        <v>0</v>
+      </c>
+      <c r="N120">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A121" s="1">
+        <v>44675</v>
+      </c>
+      <c r="B121" t="s">
+        <v>14</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121">
+        <v>3</v>
+      </c>
+      <c r="E121" t="s">
+        <v>17</v>
+      </c>
+      <c r="F121" s="2">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="G121" s="3">
+        <v>44675.635416666664</v>
+      </c>
+      <c r="H121">
+        <v>0</v>
+      </c>
+      <c r="I121">
+        <v>0</v>
+      </c>
+      <c r="J121">
+        <v>0</v>
+      </c>
+      <c r="K121">
+        <v>0</v>
+      </c>
+      <c r="L121">
+        <v>0</v>
+      </c>
+      <c r="M121">
+        <v>0</v>
+      </c>
+      <c r="N121">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A122" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B122" t="s">
+        <v>14</v>
+      </c>
+      <c r="C122">
+        <v>100</v>
+      </c>
+      <c r="D122">
+        <v>4</v>
+      </c>
+      <c r="E122" t="s">
+        <v>15</v>
+      </c>
+      <c r="F122" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="G122" s="3">
+        <v>44682.541666666664</v>
+      </c>
+      <c r="H122">
+        <v>0</v>
+      </c>
+      <c r="I122">
+        <v>0</v>
+      </c>
+      <c r="J122">
+        <v>0</v>
+      </c>
+      <c r="K122">
+        <v>0</v>
+      </c>
+      <c r="L122">
+        <v>1</v>
+      </c>
+      <c r="M122">
+        <v>0</v>
+      </c>
+      <c r="N122">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A123" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B123" t="s">
+        <v>14</v>
+      </c>
+      <c r="C123">
+        <v>100</v>
+      </c>
+      <c r="D123">
+        <v>4</v>
+      </c>
+      <c r="E123" t="s">
+        <v>16</v>
+      </c>
+      <c r="F123" s="2">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="G123" s="3">
+        <v>44682.590277777781</v>
+      </c>
+      <c r="H123">
+        <v>0</v>
+      </c>
+      <c r="I123">
+        <v>0</v>
+      </c>
+      <c r="J123">
+        <v>0</v>
+      </c>
+      <c r="K123">
+        <v>0</v>
+      </c>
+      <c r="L123">
+        <v>0</v>
+      </c>
+      <c r="M123">
+        <v>0</v>
+      </c>
+      <c r="N123">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A124" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B124" t="s">
+        <v>14</v>
+      </c>
+      <c r="C124">
+        <v>100</v>
+      </c>
+      <c r="D124">
+        <v>4</v>
+      </c>
+      <c r="E124" t="s">
+        <v>17</v>
+      </c>
+      <c r="F124" s="2">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="G124" s="3">
+        <v>44682.618055555555</v>
+      </c>
+      <c r="H124">
+        <v>0</v>
+      </c>
+      <c r="I124">
+        <v>0</v>
+      </c>
+      <c r="J124">
+        <v>0</v>
+      </c>
+      <c r="K124">
+        <v>0</v>
+      </c>
+      <c r="L124">
+        <v>0</v>
+      </c>
+      <c r="M124">
+        <v>0</v>
+      </c>
+      <c r="N124">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O37">
     <sortCondition ref="A2:A37"/>

</xml_diff>